<commit_message>
using script to update
</commit_message>
<xml_diff>
--- a/in-class-assignments/april-4/april-3-post-class-assignment.xlsx
+++ b/in-class-assignments/april-4/april-3-post-class-assignment.xlsx
@@ -63,6 +63,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -83,12 +84,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,28 +136,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -178,196 +185,196 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="3" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <v>30000</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <v>22500</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>3000</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="6" t="n">
         <f aca="false">B4-B5</f>
         <v>7500</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="6" t="n">
         <f aca="false">B$1*B4</f>
         <v>3000</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="6" t="n">
         <f aca="false">C5+D5+E5</f>
         <v>13500</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="6" t="n">
         <f aca="false">PMT(B$1,A5,-NPV(B$1, F$5:F5))</f>
         <v>13500</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>16857</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <v>4500</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="6" t="n">
         <f aca="false">B5-B6</f>
         <v>5643</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <f aca="false">B$1*B5</f>
         <v>2250</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="6" t="n">
         <f aca="false">C6+D6+E6</f>
         <v>12393</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="6" t="n">
         <f aca="false">PMT(B$1,A6,-NPV(B$1, F$5:F6))</f>
         <v>12972.8571428571</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <v>12750</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <v>7000</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <f aca="false">B6-B7</f>
         <v>4107</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="6" t="n">
         <f aca="false">B$1*B6</f>
         <v>1685.7</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="6" t="n">
         <f aca="false">C7+D7+E7</f>
         <v>12792.7</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="6" t="n">
         <f aca="false">PMT(B$1,A7,-NPV(B$1, F$5:F7))</f>
         <v>12918.4290030211</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="6" t="n">
         <v>9750</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>10000</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="6" t="n">
         <f aca="false">B7-B8</f>
         <v>3000</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="6" t="n">
         <f aca="false">B$1*B7</f>
         <v>1275</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <f aca="false">C8+D8+E8</f>
         <v>14275</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="6" t="n">
         <f aca="false">PMT(B$1,A8,-NPV(B$1, F$5:F8))</f>
         <v>13210.7304460246</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="6" t="n">
         <v>7125</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="6" t="n">
         <v>13000</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="6" t="n">
         <f aca="false">B8-B9</f>
         <v>2625</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <f aca="false">B$1*B8</f>
         <v>975</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="6" t="n">
         <f aca="false">C9+D9+E9</f>
         <v>16600</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="6" t="n">
         <f aca="false">PMT(B$1,A9,-NPV(B$1, F$5:F9))</f>
         <v>13765.8842607001</v>
       </c>

</xml_diff>